<commit_message>
7ka done and 8
</commit_message>
<xml_diff>
--- a/7/7ka.xlsx
+++ b/7/7ka.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mskrz\Desktop\Github\Fizyka-laby\7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07CEEE7-BACE-45B4-B25F-2F8CBD71EBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549432B1-6ECF-4842-B35C-2AAEEFACFCD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Zadania" sheetId="3" r:id="rId1"/>
-    <sheet name="Pomiary" sheetId="1" r:id="rId2"/>
+    <sheet name="Wyniki z zapisem" sheetId="4" r:id="rId1"/>
+    <sheet name="Zadania" sheetId="3" r:id="rId2"/>
+    <sheet name="Wykresy" sheetId="5" r:id="rId3"/>
+    <sheet name="Pomiary" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>Lp.</t>
   </si>
@@ -46,9 +48,6 @@
   </si>
   <si>
     <t>t, s</t>
-  </si>
-  <si>
-    <t>tsr, s</t>
   </si>
   <si>
     <t>odchyl</t>
@@ -159,13 +158,21 @@
     <t>RAW:</t>
   </si>
   <si>
-    <t>Zapis koncowy</t>
+    <t>1. - 6.</t>
+  </si>
+  <si>
+    <t>U(g)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -227,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -242,6 +249,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -907,7 +923,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1618,6 +1634,1363 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Wykres</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> zależności tśr(H)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>t średnia</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Zadania!$F$16:$F$25</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.0432127494016086E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.5648641138513566E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.0432127494016086E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>5.773502691896258E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>6.5648641138513566E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Zadania!$F$16:$F$25</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.0432127494016086E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.5648641138513566E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.0432127494016086E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>5.773502691896258E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>6.5648641138513566E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Zadania!$C$29</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1.7320508075688774E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Zadania!$C$29</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>1.7320508075688774E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Zadania!$C$16:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.58724999999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68724999999999992</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78725000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.88724999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98724999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.08725</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1872499999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.28725</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3872499999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.48725</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Zadania!$E$16:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.3478</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.37720000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.40200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4284</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.47400000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.49519999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.51419999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.53520000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.55460000000000009</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CE84-48D5-AC74-D41451DE9BC5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="596197560"/>
+        <c:axId val="596195400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="596197560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.5"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>H, m</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="596195400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="596195400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.30000000000000004"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>t śr,</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> s</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="596197560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>Wykres</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" baseline="0"/>
+              <a:t> zależności tśr(√H)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>t średnia</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Zadania!$F$16:$F$25</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.0432127494016086E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.5648641138513566E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.0432127494016086E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>5.773502691896258E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>6.5648641138513566E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Zadania!$F$16:$F$25</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>7.0432127494016086E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.5648641138513566E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.0432127494016086E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>5.773502691896258E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>6.3121104500264691E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>6.5648641138513566E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Zadania!$G$16:$G$25</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>1.1301058393680173E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0446558904389921E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.7605501461386598E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>9.1940662256491824E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>8.7159967671792923E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>8.3055026957278304E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7.9480308212516015E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>7.6330688803483333E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>7.3528086659744218E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>7.1013127990175642E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Zadania!$G$16:$G$25</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="10"/>
+                  <c:pt idx="0">
+                    <c:v>1.1301058393680173E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0446558904389921E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.7605501461386598E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>9.1940662256491824E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>8.7159967671792923E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>8.3055026957278304E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7.9480308212516015E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>7.6330688803483333E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>7.3528086659744218E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>7.1013127990175642E-4</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Zadania!$D$16:$D$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.76632238646668804</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82900542820900747</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.88727109724142372</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94193948850231346</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99360454910391793</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0427128080157066</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0896100219803413</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1345704032804664</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1778157750684102</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2195285974506707</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Zadania!$E$16:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.3478</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.37720000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.40200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4284</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.47400000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.49519999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.51419999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.53520000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.55460000000000009</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-26EC-4191-970C-238681D6CAF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="596197560"/>
+        <c:axId val="596195400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="596197560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.3"/>
+          <c:min val="0.70000000000000007"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>√H, √m</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="596195400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="596195400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.60000000000000009"/>
+          <c:min val="0.30000000000000004"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>t śr,</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> s</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="596197560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1698,6 +3071,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2215,6 +3668,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2787,6 +5272,87 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93B42D3C-79B5-4430-8CF0-E132DDB91C8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600364</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>173182</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD1B7C85-B1D7-47F6-874F-D4E860513708}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161635</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600364</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Wykres 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88EB8B5D-15C3-483E-A69C-943AFA23556C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3071,11 +5637,399 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A9B26B-F52B-42AC-8E7C-7341E9281569}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="7.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="str">
+        <f>Zadania!C15</f>
+        <v>H, m</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <f>Zadania!J2</f>
+        <v>odchyl</v>
+      </c>
+      <c r="F2" s="2" t="str">
+        <f>Zadania!K2</f>
+        <v>ua(tśr)</v>
+      </c>
+      <c r="G2" s="2" t="str">
+        <f>Zadania!L2</f>
+        <v>ub(tśr)</v>
+      </c>
+      <c r="H2" s="2" t="str">
+        <f>Zadania!M2</f>
+        <v>u(tśr)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!C16,RIGHT(TEXT(Zadania!$C$29,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!$C$29*10^LEN(Zadania!$C$29),2),")")</f>
+        <v>0,5873(17)</v>
+      </c>
+      <c r="C3" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!D16,RIGHT(TEXT(Zadania!G16,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!G16*10^LEN(Zadania!G16),2),")")</f>
+        <v>0,7663(11)</v>
+      </c>
+      <c r="D3" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!E16,RIGHT(TEXT(Zadania!F16,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!F16*10^LEN(Zadania!F16),2),")")</f>
+        <v>0,34780(63)</v>
+      </c>
+      <c r="E3" s="6">
+        <f>Zadania!J3</f>
+        <v>4.4721359549995833E-4</v>
+      </c>
+      <c r="F3" s="6">
+        <f>Zadania!K3</f>
+        <v>2.5513535623272624E-4</v>
+      </c>
+      <c r="G3" s="6">
+        <f>Zadania!L3</f>
+        <v>5.773502691896258E-4</v>
+      </c>
+      <c r="H3" s="6">
+        <f>Zadania!M3</f>
+        <v>6.3121104500264691E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!C17,RIGHT(TEXT(Zadania!$C$29,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!$C$29*10^LEN(Zadania!$C$29),2),")")</f>
+        <v>0,6873(17)</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!D17,RIGHT(TEXT(Zadania!G17,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!G17*10^LEN(Zadania!G17),2),")")</f>
+        <v>0,8290(10)</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!E17,RIGHT(TEXT(Zadania!F17,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!F17*10^LEN(Zadania!F17),2),")")</f>
+        <v>0,37720(63)</v>
+      </c>
+      <c r="E4" s="6">
+        <f>Zadania!J4</f>
+        <v>4.4721359549995833E-4</v>
+      </c>
+      <c r="F4" s="6">
+        <f>Zadania!K4</f>
+        <v>2.5513535623272624E-4</v>
+      </c>
+      <c r="G4" s="6">
+        <f>Zadania!L4</f>
+        <v>5.773502691896258E-4</v>
+      </c>
+      <c r="H4" s="6">
+        <f>Zadania!M4</f>
+        <v>6.3121104500264691E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!C18,RIGHT(TEXT(Zadania!$C$29,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!$C$29*10^LEN(Zadania!$C$29),2),")")</f>
+        <v>0,7873(17)</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!D18,RIGHT(TEXT(Zadania!G18,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!G18*10^LEN(Zadania!G18),2),")")</f>
+        <v>0,88727(97)</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!E18,RIGHT(TEXT(Zadania!F18,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!F18*10^LEN(Zadania!F18),2),")")</f>
+        <v>0,40200(70)</v>
+      </c>
+      <c r="E5" s="6">
+        <f>Zadania!J5</f>
+        <v>7.0710678118654816E-4</v>
+      </c>
+      <c r="F5" s="6">
+        <f>Zadania!K5</f>
+        <v>4.0340441866692573E-4</v>
+      </c>
+      <c r="G5" s="6">
+        <f>Zadania!L5</f>
+        <v>5.773502691896258E-4</v>
+      </c>
+      <c r="H5" s="6">
+        <f>Zadania!M5</f>
+        <v>7.0432127494016086E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!C19,RIGHT(TEXT(Zadania!$C$29,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!$C$29*10^LEN(Zadania!$C$29),2),")")</f>
+        <v>0,8873(17)</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!D19,RIGHT(TEXT(Zadania!G19,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!G19*10^LEN(Zadania!G19),2),")")</f>
+        <v>0,94194(91)</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!E19,RIGHT(TEXT(Zadania!F19,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!F19*10^LEN(Zadania!F19),2),")")</f>
+        <v>0,42840(65)</v>
+      </c>
+      <c r="E6" s="6">
+        <f>Zadania!J6</f>
+        <v>5.4772255750516654E-4</v>
+      </c>
+      <c r="F6" s="6">
+        <f>Zadania!K6</f>
+        <v>3.1247571905669753E-4</v>
+      </c>
+      <c r="G6" s="6">
+        <f>Zadania!L6</f>
+        <v>5.773502691896258E-4</v>
+      </c>
+      <c r="H6" s="6">
+        <f>Zadania!M6</f>
+        <v>6.5648641138513566E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!C20,RIGHT(TEXT(Zadania!$C$29,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!$C$29*10^LEN(Zadania!$C$29),2),")")</f>
+        <v>0,9873(17)</v>
+      </c>
+      <c r="C7" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!D20,RIGHT(TEXT(Zadania!G20,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!G20*10^LEN(Zadania!G20),2),")")</f>
+        <v>0,99360(87)</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!E20,RIGHT(TEXT(Zadania!F20,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!F20*10^LEN(Zadania!F20),2),")")</f>
+        <v>0,45300(70)</v>
+      </c>
+      <c r="E7" s="6">
+        <f>Zadania!J7</f>
+        <v>7.0710678118654816E-4</v>
+      </c>
+      <c r="F7" s="6">
+        <f>Zadania!K7</f>
+        <v>4.0340441866692573E-4</v>
+      </c>
+      <c r="G7" s="6">
+        <f>Zadania!L7</f>
+        <v>5.773502691896258E-4</v>
+      </c>
+      <c r="H7" s="6">
+        <f>Zadania!M7</f>
+        <v>7.0432127494016086E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!C21,RIGHT(TEXT(Zadania!$C$29,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!$C$29*10^LEN(Zadania!$C$29),2),")")</f>
+        <v>1,0873(17)</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!D21,RIGHT(TEXT(Zadania!G21,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!G21*10^LEN(Zadania!G21),2),")")</f>
+        <v>1,04271(83)</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!E21,RIGHT(TEXT(Zadania!F21,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!F21*10^LEN(Zadania!F21),2),")")</f>
+        <v>0,47400(57)</v>
+      </c>
+      <c r="E8" s="6">
+        <f>Zadania!J8</f>
+        <v>6.2063353831181828E-17</v>
+      </c>
+      <c r="F8" s="6">
+        <f>Zadania!K8</f>
+        <v>3.5407143360689232E-17</v>
+      </c>
+      <c r="G8" s="6">
+        <f>Zadania!L8</f>
+        <v>5.773502691896258E-4</v>
+      </c>
+      <c r="H8" s="6">
+        <f>Zadania!M8</f>
+        <v>5.773502691896258E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!C22,RIGHT(TEXT(Zadania!$C$29,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!$C$29*10^LEN(Zadania!$C$29),2),")")</f>
+        <v>1,1873(17)</v>
+      </c>
+      <c r="C9" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!D22,RIGHT(TEXT(Zadania!G22,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!G22*10^LEN(Zadania!G22),2),")")</f>
+        <v>1,08961(79)</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!E22,RIGHT(TEXT(Zadania!F22,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!F22*10^LEN(Zadania!F22),2),")")</f>
+        <v>0,49520(63)</v>
+      </c>
+      <c r="E9" s="6">
+        <f>Zadania!J9</f>
+        <v>4.4721359549995833E-4</v>
+      </c>
+      <c r="F9" s="6">
+        <f>Zadania!K9</f>
+        <v>2.5513535623272624E-4</v>
+      </c>
+      <c r="G9" s="6">
+        <f>Zadania!L9</f>
+        <v>5.773502691896258E-4</v>
+      </c>
+      <c r="H9" s="6">
+        <f>Zadania!M9</f>
+        <v>6.3121104500264691E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!C23,RIGHT(TEXT(Zadania!$C$29,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!$C$29*10^LEN(Zadania!$C$29),2),")")</f>
+        <v>1,2873(17)</v>
+      </c>
+      <c r="C10" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!D23,RIGHT(TEXT(Zadania!G23,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!G23*10^LEN(Zadania!G23),2),")")</f>
+        <v>1,13457(76)</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!E23,RIGHT(TEXT(Zadania!F23,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!F23*10^LEN(Zadania!F23),2),")")</f>
+        <v>0,51420(63)</v>
+      </c>
+      <c r="E10" s="6">
+        <f>Zadania!J10</f>
+        <v>4.4721359549995833E-4</v>
+      </c>
+      <c r="F10" s="6">
+        <f>Zadania!K10</f>
+        <v>2.5513535623272624E-4</v>
+      </c>
+      <c r="G10" s="6">
+        <f>Zadania!L10</f>
+        <v>5.773502691896258E-4</v>
+      </c>
+      <c r="H10" s="6">
+        <f>Zadania!M10</f>
+        <v>6.3121104500264691E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="8" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!C24,RIGHT(TEXT(Zadania!$C$29,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!$C$29*10^LEN(Zadania!$C$29),2),")")</f>
+        <v>1,3873(17)</v>
+      </c>
+      <c r="C11" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!D24,RIGHT(TEXT(Zadania!G24,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!G24*10^LEN(Zadania!G24),2),")")</f>
+        <v>1,17782(73)</v>
+      </c>
+      <c r="D11" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!E24,RIGHT(TEXT(Zadania!F24,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!F24*10^LEN(Zadania!F24),2),")")</f>
+        <v>0,53520(63)</v>
+      </c>
+      <c r="E11" s="6">
+        <f>Zadania!J11</f>
+        <v>4.4721359549995833E-4</v>
+      </c>
+      <c r="F11" s="6">
+        <f>Zadania!K11</f>
+        <v>2.5513535623272624E-4</v>
+      </c>
+      <c r="G11" s="6">
+        <f>Zadania!L11</f>
+        <v>5.773502691896258E-4</v>
+      </c>
+      <c r="H11" s="6">
+        <f>Zadania!M11</f>
+        <v>6.3121104500264691E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!C25,RIGHT(TEXT(Zadania!$C$29,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!$C$29*10^LEN(Zadania!$C$29),2),")")</f>
+        <v>1,4873(17)</v>
+      </c>
+      <c r="C12" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!D25,RIGHT(TEXT(Zadania!G25,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!G25*10^LEN(Zadania!G25),2),")")</f>
+        <v>1,21953(71)</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f>_xlfn.CONCAT(FIXED(Zadania!E25,RIGHT(TEXT(Zadania!F25,"0,00E+00"),2)+1,TRUE),"(",LEFT(Zadania!F25*10^LEN(Zadania!F25),2),")")</f>
+        <v>0,55460(65)</v>
+      </c>
+      <c r="E12" s="6">
+        <f>Zadania!J12</f>
+        <v>5.4772255750516665E-4</v>
+      </c>
+      <c r="F12" s="6">
+        <f>Zadania!K12</f>
+        <v>3.1247571905669759E-4</v>
+      </c>
+      <c r="G12" s="6">
+        <f>Zadania!L12</f>
+        <v>5.773502691896258E-4</v>
+      </c>
+      <c r="H12" s="6">
+        <f>Zadania!M12</f>
+        <v>6.5648641138513566E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A460A7-3949-42AF-A0E0-AAEB0C0F0D08}">
   <dimension ref="B1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6:Q10"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3085,8 +6039,9 @@
     <col min="4" max="4" width="14.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.1796875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
@@ -3104,16 +6059,16 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.35">
@@ -3150,22 +6105,22 @@
         <v>tśr, s</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.35">
@@ -3222,7 +6177,7 @@
         <v>0,34780(63)</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q3" s="1">
         <v>1.141</v>
@@ -3258,7 +6213,7 @@
         <v>0.377</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" ref="I4:I13" si="0">AVERAGE(D4:H4)</f>
+        <f t="shared" ref="I4:I12" si="0">AVERAGE(D4:H4)</f>
         <v>0.37720000000000004</v>
       </c>
       <c r="J4" s="2">
@@ -3390,7 +6345,7 @@
         <v>0,42840(65)</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.35">
@@ -3719,36 +6674,36 @@
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.35">
       <c r="N13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="O14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="Q14" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.35">
@@ -3759,28 +6714,28 @@
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O15" s="2">
+      <c r="O15" s="7">
         <f>2/I16^2</f>
         <v>9.6772962155157476</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P15" s="7">
         <f>ABS(-4*I17/I16^3)</f>
         <v>8.2837514871995921E-2</v>
       </c>
@@ -3813,15 +6768,15 @@
         <f>$C$29/2/D16</f>
         <v>1.1301058393680173E-3</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="7">
         <f t="array" ref="I16:J18">LINEST(E16:E25,D16:D25,TRUE,TRUE)</f>
         <v>0.45460894888770187</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="7">
         <v>-1.9404265393496711E-4</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B17" s="2">
         <v>2</v>
       </c>
@@ -3846,22 +6801,22 @@
         <v>1.0446558904389921E-3</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" s="2">
+        <v>19</v>
+      </c>
+      <c r="I17" s="7">
         <v>1.945722995646694E-3</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="7">
         <v>1.981630752785811E-3</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B18" s="2">
         <v>3</v>
       </c>
@@ -3886,16 +6841,19 @@
         <v>9.7605501461386598E-4</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18" s="2">
+        <v>20</v>
+      </c>
+      <c r="I18" s="7">
         <v>0.9998534747707265</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="7">
         <v>8.8537929515664679E-4</v>
       </c>
+      <c r="P18" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B19" s="2">
         <v>4</v>
       </c>
@@ -3919,8 +6877,12 @@
         <f t="shared" si="10"/>
         <v>9.1940662256491824E-4</v>
       </c>
+      <c r="P19" s="1">
+        <f>P15*2</f>
+        <v>0.16567502974399184</v>
+      </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B20" s="2">
         <v>5</v>
       </c>
@@ -3944,8 +6906,12 @@
         <f t="shared" si="10"/>
         <v>8.7159967671792923E-4</v>
       </c>
+      <c r="I20" s="1" t="str">
+        <f>_xlfn.CONCAT(FIXED(I16,RIGHT(TEXT(I17,"0,00E+00"),2)+1,TRUE),"(",LEFT(I17*10^LEN(I17),2),")")</f>
+        <v>0,4546(19)</v>
+      </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B21" s="2">
         <v>6</v>
       </c>
@@ -3970,7 +6936,7 @@
         <v>8.3055026957278304E-4</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B22" s="2">
         <v>7</v>
       </c>
@@ -3995,7 +6961,7 @@
         <v>7.9480308212516015E-4</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B23" s="2">
         <v>8</v>
       </c>
@@ -4020,7 +6986,7 @@
         <v>7.6330688803483333E-4</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B24" s="2">
         <v>9</v>
       </c>
@@ -4045,7 +7011,7 @@
         <v>7.3528086659744218E-4</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B25" s="2">
         <v>10</v>
       </c>
@@ -4070,21 +7036,21 @@
         <v>7.1013127990175642E-4</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B29" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="5">
         <f>0.003/SQRT(3)</f>
         <v>1.7320508075688774E-3</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -4094,7 +7060,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24017ECE-478E-4E20-91F1-5BB7C4B9D999}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
@@ -4113,7 +7095,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -4150,7 +7132,7 @@
         <v>5</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -4435,7 +7417,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>2</v>
@@ -4468,7 +7450,7 @@
         <v>5</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>